<commit_message>
Kommit en bit med Blackbox, se om jag kan hitta mer fel
</commit_message>
<xml_diff>
--- a/Blackbox Testfall.xlsx
+++ b/Blackbox Testfall.xlsx
@@ -8,16 +8,97 @@
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
-    <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+  <si>
+    <t>Testfall</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Förväntad output</t>
+  </si>
+  <si>
+    <t>Resultat</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>"Triangeln är liksidig"</t>
+  </si>
+  <si>
+    <t>Lyckat</t>
+  </si>
+  <si>
+    <t>"Triangeln har inga lika sidor"</t>
+  </si>
+  <si>
+    <t>1,0 4,0 4,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Trianglen är likbent" </t>
+  </si>
+  <si>
+    <t>Stämmer</t>
+  </si>
+  <si>
+    <t>Triangeln har inga lika sidor</t>
+  </si>
+  <si>
+    <t>Ett felmeddelande</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>4.0 4.0 4.0</t>
+  </si>
+  <si>
+    <t>3.0 2.0 1.0</t>
+  </si>
+  <si>
+    <t>4.5 4.5 4.5</t>
+  </si>
+  <si>
+    <t>3.3 2.2 1.1</t>
+  </si>
+  <si>
+    <t>1.1 4.4 4.4</t>
+  </si>
+  <si>
+    <t>0.4 0.7 1.0</t>
+  </si>
+  <si>
+    <t>1.0- 1.0- 1.0-</t>
+  </si>
+  <si>
+    <t>2.0 2.0</t>
+  </si>
+  <si>
+    <t>2.0 2.0 2.0 2.0</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>System.FormatException</t>
+  </si>
+  <si>
+    <t>ASDF</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,13 +106,86 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="4"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -43,14 +197,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bra" xfId="2" builtinId="26"/>
+    <cellStyle name="Dålig" xfId="3" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Rubrik" xfId="1" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -342,38 +519,327 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22.5">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Tror jag är klar med Testfall nu måste jag skriva kommentarer och rapport
</commit_message>
<xml_diff>
--- a/Blackbox Testfall.xlsx
+++ b/Blackbox Testfall.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>Testfall</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t>ASDF</t>
+  </si>
+  <si>
+    <t>1.0 -2.0 3.0</t>
+  </si>
+  <si>
+    <t>´-1.0 2.0 3.0</t>
+  </si>
+  <si>
+    <t>1.244 1.2 1.49</t>
   </si>
 </sst>
 </file>
@@ -203,10 +212,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -216,12 +224,19 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bra" xfId="2" builtinId="26"/>
@@ -519,42 +534,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -563,109 +578,109 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="15.75">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -674,31 +689,31 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+      <c r="C9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -707,40 +722,40 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="C11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -749,29 +764,29 @@
       <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="11" t="s">
+      <c r="C14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -780,54 +795,84 @@
       <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="6">
+      <c r="B16" s="11">
+        <v>987</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="6">
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="6">
+      <c r="B18" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="6">
-        <v>19</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="6">
-        <v>20</v>
-      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Rapport kvar sen whitebox
</commit_message>
<xml_diff>
--- a/Blackbox Testfall.xlsx
+++ b/Blackbox Testfall.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>Testfall</t>
   </si>
@@ -101,13 +101,55 @@
   </si>
   <si>
     <t>1.244 1.2 1.49</t>
+  </si>
+  <si>
+    <t>1.0 2.0 -3.0</t>
+  </si>
+  <si>
+    <t>(Mellanslag)</t>
+  </si>
+  <si>
+    <t>(Tom)</t>
+  </si>
+  <si>
+    <t>Något fel med avrundingen</t>
+  </si>
+  <si>
+    <t>Kraschar det</t>
+  </si>
+  <si>
+    <t>—〃—</t>
+  </si>
+  <si>
+    <t>Tar in tal Under 0</t>
+  </si>
+  <si>
+    <t>Tar in allt förutom string verkar det som</t>
+  </si>
+  <si>
+    <t>Vad händer med det fjärde talet?</t>
+  </si>
+  <si>
+    <t>Tar in Whitespace</t>
+  </si>
+  <si>
+    <t>Storleken eller att det bara är ett tal spelar ingen roll</t>
+  </si>
+  <si>
+    <t>Tittar om den tar hand om tal olika på olika ställen</t>
+  </si>
+  <si>
+    <t>Tar inte hand om null</t>
+  </si>
+  <si>
+    <t>Tar inte hand om whitespace</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,12 +180,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="4"/>
@@ -162,6 +198,33 @@
     <font>
       <sz val="11"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -212,31 +275,30 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bra" xfId="2" builtinId="26"/>
@@ -537,94 +599,97 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="5">
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75">
-      <c r="A3" s="5">
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="17.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="8"/>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="5">
+      <c r="F3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="5">
+      <c r="F4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -634,34 +699,35 @@
         <v>5</v>
       </c>
       <c r="D5" s="8"/>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="15"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="5">
+      <c r="F5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="5">
+      <c r="F6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -671,32 +737,35 @@
         <v>9</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="15"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="5">
+      <c r="F7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="12"/>
+      <c r="F8" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="5">
+    <row r="9" spans="1:7" ht="15.75">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -706,173 +775,242 @@
         <v>12</v>
       </c>
       <c r="D9" s="8"/>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="16">
+        <v>987</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="9" t="s">
+      <c r="F16" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="11">
-        <v>987</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="5">
-        <v>17</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="5">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="16"/>
+      <c r="F20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>